<commit_message>
Meanwhile don't use PS's Model (PS_IDTest)
</commit_message>
<xml_diff>
--- a/Docs/BOM.ETX2i10G.xlsx
+++ b/Docs/BOM.ETX2i10G.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\ate\AutoTesters\TCL\ETX-2i-10G\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7CAB08-118A-4333-85EB-7385B9485F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B443BF2-5D0D-4192-B961-BA1DE1E1F19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5205" yWindow="480" windowWidth="21945" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38940" yWindow="1860" windowWidth="17025" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -991,7 +991,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1020,21 +1020,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1057,7 +1042,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1067,71 +1052,79 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1155,423 +1148,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1697,30 +1273,30 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
+        <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1736,16 +1312,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1893,32 +1459,23 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2059,26 +1616,64 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
+        <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2200,6 +1795,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -2207,20 +1818,99 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2252,6 +1942,82 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="7"/>
         <color theme="1"/>
         <name val="Times New Roman"/>
@@ -2271,6 +2037,119 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="7"/>
         <color theme="1"/>
         <name val="Times New Roman"/>
@@ -2278,6 +2157,120 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2315,40 +2308,40 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BE738A19-B3FF-4F52-AF6A-0EFC9F0E4E48}" name="Table1" displayName="Table1" ref="A29:F44" totalsRowShown="0" headerRowDxfId="54">
   <autoFilter ref="A29:F44" xr:uid="{BE738A19-B3FF-4F52-AF6A-0EFC9F0E4E48}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A59F7AB7-C798-4628-B193-917426F1FB7B}" name=" 3.2.    Specify cables:" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{6FE1CF3B-7F91-420F-B9A0-8F90D31F5C39}" name=" 2 units" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{9E1AAFA9-80BD-4E73-82CF-B0A99E9A3782}" name="OutDoor_x000a_(4 units)" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{BFCC9EAF-5C56-4874-A85C-3B4471661E39}" name="MainBoard_x000a_(2 units)" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{981D7326-ADE8-4669-B02B-6D2CD54EBB17}" name="Column1" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{54C2621F-9D69-43F3-8271-49B9B5A1C971}" name="Column2" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A59F7AB7-C798-4628-B193-917426F1FB7B}" name=" 3.2.    Specify cables:" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{6FE1CF3B-7F91-420F-B9A0-8F90D31F5C39}" name=" 2 units" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{9E1AAFA9-80BD-4E73-82CF-B0A99E9A3782}" name="OutDoor_x000a_(4 units)" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{BFCC9EAF-5C56-4874-A85C-3B4471661E39}" name="MainBoard_x000a_(2 units)" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{981D7326-ADE8-4669-B02B-6D2CD54EBB17}" name="Column1" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{54C2621F-9D69-43F3-8271-49B9B5A1C971}" name="Column2" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{283AB01A-3A5F-47F6-9ECD-E5EB5737E221}" name="Table2" displayName="Table2" ref="A18:F27" totalsRowShown="0" headerRowDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{283AB01A-3A5F-47F6-9ECD-E5EB5737E221}" name="Table2" displayName="Table2" ref="A18:F27" totalsRowShown="0" headerRowDxfId="47">
   <autoFilter ref="A18:F27" xr:uid="{283AB01A-3A5F-47F6-9ECD-E5EB5737E221}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{3091BF04-D61A-4553-8079-5E5EC3709299}" name="3.1.    RAD cables:" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{470B0302-3602-4FE9-A495-1D964C68B563}" name=" 2 units" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{C96E22D6-0264-4BDE-AEA3-B885133A4CA4}" name="OutDoor_x000a_(4 units)" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{7386AD56-DD53-4EA8-96AA-689BC05E8414}" name="MainBoard_x000a_(2 units)" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{967DF8E1-4280-41D9-8159-B45114BF9269}" name="Column1" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{C7DB5F3B-C59D-4C3F-BBA5-83C4FBBD1257}" name="Column2" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{3091BF04-D61A-4553-8079-5E5EC3709299}" name="3.1.    RAD cables:" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{470B0302-3602-4FE9-A495-1D964C68B563}" name=" 2 units" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{C96E22D6-0264-4BDE-AEA3-B885133A4CA4}" name="OutDoor_x000a_(4 units)" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{7386AD56-DD53-4EA8-96AA-689BC05E8414}" name="MainBoard_x000a_(2 units)" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{967DF8E1-4280-41D9-8159-B45114BF9269}" name="Column1" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{C7DB5F3B-C59D-4C3F-BBA5-83C4FBBD1257}" name="Column2" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F45989F9-C4FE-46C3-9118-DBF76BDD6F2C}" name="Table3" displayName="Table3" ref="A4:F11" totalsRowShown="0" headerRowDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F45989F9-C4FE-46C3-9118-DBF76BDD6F2C}" name="Table3" displayName="Table3" ref="A4:F11" totalsRowShown="0" headerRowDxfId="40">
   <autoFilter ref="A4:F11" xr:uid="{F45989F9-C4FE-46C3-9118-DBF76BDD6F2C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D19D5E56-B2A0-4A39-A688-183835D9C627}" name=" 1.       RAD products:" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{654FC895-C041-424B-9EF2-3E199BD9726B}" name=" 2 units" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{246DFA9C-98F6-476B-8752-28605A484844}" name="OutDoor_x000a_(4 units)" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{379E9E9F-7E5E-4731-9EB8-3E2652170E79}" name="MainBoard_x000a_(2 units)" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{D19D5E56-B2A0-4A39-A688-183835D9C627}" name=" 1.       RAD products:" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{654FC895-C041-424B-9EF2-3E199BD9726B}" name=" 2 units" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{246DFA9C-98F6-476B-8752-28605A484844}" name="OutDoor_x000a_(4 units)" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{379E9E9F-7E5E-4731-9EB8-3E2652170E79}" name="MainBoard_x000a_(2 units)" dataDxfId="36"/>
     <tableColumn id="5" xr3:uid="{4E2E51EC-8011-4B7E-B1BA-31B47C897C7A}" name="Column1"/>
     <tableColumn id="6" xr3:uid="{629A07B3-D61D-476C-A66E-10B5F08E4C40}" name="Column2"/>
   </tableColumns>
@@ -2357,67 +2350,67 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2E083F03-EA1C-4C79-927F-7B71E88FBF35}" name="Table5" displayName="Table5" ref="A12:F15" totalsRowShown="0" headerRowDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2E083F03-EA1C-4C79-927F-7B71E88FBF35}" name="Table5" displayName="Table5" ref="A12:F15" totalsRowShown="0" headerRowDxfId="35">
   <autoFilter ref="A12:F15" xr:uid="{2E083F03-EA1C-4C79-927F-7B71E88FBF35}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{F33DBF42-4C3C-4800-AE5C-9240897E0E92}" name="2.       A.T.E. products:"/>
-    <tableColumn id="2" xr3:uid="{FD9D604A-97B3-4258-8243-5530B17E3C16}" name=" 2 units" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{F62D2983-9A37-4A91-BE59-498E99BB8C9A}" name="OutDoor_x000a_(4 units)" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{F775654E-6625-44DB-B171-45EE431F1F1B}" name="MainBoard_x000a_(2 units)" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{88949219-7CDA-4321-95D2-431985FEF64E}" name="Column1" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{CFAE3617-231C-440A-9814-3491ADD1E5F7}" name="Column2" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{FD9D604A-97B3-4258-8243-5530B17E3C16}" name=" 2 units" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{F62D2983-9A37-4A91-BE59-498E99BB8C9A}" name="OutDoor_x000a_(4 units)" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{F775654E-6625-44DB-B171-45EE431F1F1B}" name="MainBoard_x000a_(2 units)" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{88949219-7CDA-4321-95D2-431985FEF64E}" name="Column1" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{CFAE3617-231C-440A-9814-3491ADD1E5F7}" name="Column2" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{29747EB6-9D7A-4AA7-AAD7-923DDA372A6C}" name="Table6" displayName="Table6" ref="A46:D49" totalsRowShown="0" headerRowBorderDxfId="49" tableBorderDxfId="50" totalsRowBorderDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{29747EB6-9D7A-4AA7-AAD7-923DDA372A6C}" name="Table6" displayName="Table6" ref="A46:D49" totalsRowShown="0" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
   <autoFilter ref="A46:D49" xr:uid="{29747EB6-9D7A-4AA7-AAD7-923DDA372A6C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{479E1687-5AC7-4BA3-8758-214A4B6A5504}" name="4.       Mechanic parts:" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{8252F755-5C3A-49F2-AB21-7657822BDCEE}" name=" 2 units" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{966CF58A-3752-4D41-AECE-920E581465A8}" name="OutDoor_x000a_(4 units)" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{DC9384FE-EBDA-4440-8CF5-2BD783C14C79}" name="MainBoard_x000a_(2 units)" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{479E1687-5AC7-4BA3-8758-214A4B6A5504}" name="4.       Mechanic parts:" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{8252F755-5C3A-49F2-AB21-7657822BDCEE}" name=" 2 units" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{966CF58A-3752-4D41-AECE-920E581465A8}" name="OutDoor_x000a_(4 units)" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{DC9384FE-EBDA-4440-8CF5-2BD783C14C79}" name="MainBoard_x000a_(2 units)" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2940D1D2-1742-448B-BC6C-C654E9E16A3E}" name="Table7" displayName="Table7" ref="A54:D59" totalsRowShown="0" headerRowDxfId="35" dataDxfId="36" headerRowBorderDxfId="42" tableBorderDxfId="43" totalsRowBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2940D1D2-1742-448B-BC6C-C654E9E16A3E}" name="Table7" displayName="Table7" ref="A54:D59" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <autoFilter ref="A54:D59" xr:uid="{2940D1D2-1742-448B-BC6C-C654E9E16A3E}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{42289E71-A17F-4FD2-B9A7-AC6C60B88EC6}" name="5.2.    Movable equipment" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{E9E477FC-42DE-4DAD-A88A-A278C9AD03E0}" name=" 2 units" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{644E8A87-5916-4235-ADA8-03E6E4ACE1DF}" name="OutDoor_x000a_(4 units)" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{7B1AC115-3A38-4AAD-8756-613AB5C23BCF}" name="MainBoard_x000a_(2 units)" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{42289E71-A17F-4FD2-B9A7-AC6C60B88EC6}" name="5.2.    Movable equipment" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{E9E477FC-42DE-4DAD-A88A-A278C9AD03E0}" name=" 2 units" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{644E8A87-5916-4235-ADA8-03E6E4ACE1DF}" name="OutDoor_x000a_(4 units)" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{7B1AC115-3A38-4AAD-8756-613AB5C23BCF}" name="MainBoard_x000a_(2 units)" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{308EC0D6-A130-4F10-9F7D-F559D1D64F90}" name="Table8" displayName="Table8" ref="A52:D53" totalsRowShown="0" headerRowDxfId="29" tableBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{308EC0D6-A130-4F10-9F7D-F559D1D64F90}" name="Table8" displayName="Table8" ref="A52:D53" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="A52:D53" xr:uid="{308EC0D6-A130-4F10-9F7D-F559D1D64F90}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83AF3E1C-0C53-4E3A-8FFB-089ED9175552}" name="5.1.    PC’s card" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{FA742A23-1518-4231-A7F2-20B45E8F818C}" name=" 2 units" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{CE72879D-53C3-4889-A817-03F5BA259673}" name="OutDoor_x000a_(4 units)" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{AFBD13EF-A425-4823-8034-167E8A70D966}" name="MainBoard_x000a_(2 units)" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{83AF3E1C-0C53-4E3A-8FFB-089ED9175552}" name="5.1.    PC’s card" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{FA742A23-1518-4231-A7F2-20B45E8F818C}" name=" 2 units" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{CE72879D-53C3-4889-A817-03F5BA259673}" name="OutDoor_x000a_(4 units)" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{AFBD13EF-A425-4823-8034-167E8A70D966}" name="MainBoard_x000a_(2 units)" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{52632D65-FA75-4174-A90B-5C8B0A320A97}" name="Table9" displayName="Table9" ref="A68:D74" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="27" tableBorderDxfId="28" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{52632D65-FA75-4174-A90B-5C8B0A320A97}" name="Table9" displayName="Table9" ref="A68:D74" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="A68:D74" xr:uid="{52632D65-FA75-4174-A90B-5C8B0A320A97}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A60CF906-F771-47E1-92CE-46638A38F534}" name="7.       Miscellaneous:" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{5297B3B9-9B20-4BC3-9B9C-1B7F0C644436}" name=" 2 units" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{733D28BC-FC5B-40D6-B771-2879FD332E09}" name="OutDoor_x000a_(4 units)" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{C96522C0-1CEC-4E3C-B82C-D87E9AA546C2}" name="MainBoard_x000a_(2 units)" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{A60CF906-F771-47E1-92CE-46638A38F534}" name="7.       Miscellaneous:" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{5297B3B9-9B20-4BC3-9B9C-1B7F0C644436}" name=" 2 units" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{733D28BC-FC5B-40D6-B771-2879FD332E09}" name="OutDoor_x000a_(4 units)" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{C96522C0-1CEC-4E3C-B82C-D87E9AA546C2}" name="MainBoard_x000a_(2 units)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2686,10 +2679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2700,698 +2693,679 @@
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-    </row>
-    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E3" s="49" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="37" t="s">
         <v>71</v>
       </c>
       <c r="F3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="7">
         <v>1</v>
       </c>
-      <c r="C5" s="29">
-        <v>0</v>
-      </c>
-      <c r="D5" s="29">
-        <v>0</v>
-      </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-    </row>
-    <row r="6" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="7">
         <v>6</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="7">
         <v>10</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="7">
         <v>10</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="7">
         <v>2</v>
       </c>
-      <c r="C7" s="29">
-        <v>0</v>
-      </c>
-      <c r="D7" s="29">
-        <v>0</v>
-      </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-    </row>
-    <row r="8" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="7">
         <v>2</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="7">
         <f t="shared" ref="C8:C56" si="0">B8*2</f>
         <v>4</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="7">
         <v>2</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-    </row>
-    <row r="9" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+    </row>
+    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="7">
         <v>1</v>
       </c>
-      <c r="C9" s="29">
-        <v>0</v>
-      </c>
-      <c r="D9" s="29">
-        <v>0</v>
-      </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="7">
         <v>1</v>
       </c>
-      <c r="C10" s="29">
-        <v>0</v>
-      </c>
-      <c r="D10" s="29">
-        <v>0</v>
-      </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="7">
         <v>4</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="7">
         <v>8</v>
       </c>
-      <c r="D11" s="29">
-        <v>0</v>
-      </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-    </row>
-    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="47" t="s">
+      <c r="E12" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="47" t="s">
+      <c r="F12" s="22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="7">
         <v>2</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="7">
         <v>2</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="29">
+      <c r="B14" s="7">
         <v>1</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="7">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="7">
         <v>1</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="45" t="s">
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="7">
         <v>2</v>
       </c>
-      <c r="C15" s="29">
-        <v>0</v>
-      </c>
-      <c r="D15" s="29">
+      <c r="C15" s="7">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7">
         <v>0</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="46"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="29"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="35"/>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-    </row>
-    <row r="18" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="47" t="s">
+      <c r="E18" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="47" t="s">
+      <c r="F18" s="22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
+    <row r="19" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="7">
         <v>4</v>
       </c>
-      <c r="C19" s="29">
+      <c r="C19" s="7">
         <v>4</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="7">
         <v>0</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
+    <row r="20" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="29">
+      <c r="B20" s="7">
         <v>21</v>
       </c>
-      <c r="C20" s="29">
+      <c r="C20" s="7">
         <v>1</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D20" s="7">
         <v>3</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+    <row r="21" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="29">
+      <c r="B21" s="7">
         <v>2</v>
       </c>
-      <c r="C21" s="29">
-        <v>0</v>
-      </c>
-      <c r="D21" s="29">
+      <c r="C21" s="7">
+        <v>0</v>
+      </c>
+      <c r="D21" s="7">
         <v>0</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+    <row r="22" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="29">
+      <c r="B22" s="7">
         <v>2</v>
       </c>
-      <c r="C22" s="29">
-        <v>0</v>
-      </c>
-      <c r="D22" s="29">
+      <c r="C22" s="7">
+        <v>0</v>
+      </c>
+      <c r="D22" s="7">
         <v>0</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
+    <row r="23" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="29">
+      <c r="B23" s="7">
         <v>1</v>
       </c>
-      <c r="C23" s="29">
-        <v>0</v>
-      </c>
-      <c r="D23" s="29">
+      <c r="C23" s="7">
+        <v>0</v>
+      </c>
+      <c r="D23" s="7">
         <v>0</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
+    <row r="24" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="29">
+      <c r="B24" s="7">
         <v>1</v>
       </c>
-      <c r="C24" s="29">
+      <c r="C24" s="7">
         <v>5</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D24" s="7">
         <v>1</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
+    <row r="25" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="29">
+      <c r="B25" s="7">
         <v>2</v>
       </c>
-      <c r="C25" s="29">
+      <c r="C25" s="7">
         <v>8</v>
       </c>
-      <c r="D25" s="29">
+      <c r="D25" s="7">
         <v>2</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+    <row r="26" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="29">
+      <c r="B26" s="7">
         <v>2</v>
       </c>
-      <c r="C26" s="29">
+      <c r="C26" s="7">
         <v>4</v>
       </c>
-      <c r="D26" s="29">
+      <c r="D26" s="7">
         <v>2</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
+    <row r="27" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="29">
+      <c r="B27" s="7">
         <v>2</v>
       </c>
-      <c r="C27" s="29">
-        <v>0</v>
-      </c>
-      <c r="D27" s="29">
+      <c r="C27" s="7">
+        <v>0</v>
+      </c>
+      <c r="D27" s="7">
         <v>2</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-    </row>
-    <row r="29" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="43" t="s">
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="44" t="s">
+      <c r="C29" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="44" t="s">
+      <c r="D29" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E29" s="47" t="s">
+      <c r="E29" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F29" s="47" t="s">
+      <c r="F29" s="22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="29">
+      <c r="B30" s="7">
         <v>1</v>
       </c>
-      <c r="C30" s="29">
+      <c r="C30" s="7">
         <v>2</v>
       </c>
-      <c r="D30" s="29">
+      <c r="D30" s="7">
         <v>1</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="29">
+      <c r="B31" s="7">
         <v>2</v>
       </c>
-      <c r="C31" s="29">
-        <v>0</v>
-      </c>
-      <c r="D31" s="29">
+      <c r="C31" s="7">
+        <v>0</v>
+      </c>
+      <c r="D31" s="7">
         <v>0</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
+    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="29">
+      <c r="B32" s="7">
         <v>2</v>
       </c>
-      <c r="C32" s="29">
-        <v>0</v>
-      </c>
-      <c r="D32" s="29">
+      <c r="C32" s="7">
+        <v>0</v>
+      </c>
+      <c r="D32" s="7">
         <v>0</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="29">
+      <c r="B33" s="7">
         <v>4</v>
       </c>
-      <c r="C33" s="29">
+      <c r="C33" s="7">
         <v>8</v>
       </c>
-      <c r="D33" s="29">
+      <c r="D33" s="7">
         <v>0</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="29">
+      <c r="B34" s="7">
         <v>2</v>
       </c>
-      <c r="C34" s="29">
-        <v>0</v>
-      </c>
-      <c r="D34" s="29">
+      <c r="C34" s="7">
+        <v>0</v>
+      </c>
+      <c r="D34" s="7">
         <v>0</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="30" t="s">
+      <c r="A35" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="29">
+      <c r="B35" s="7">
         <v>6</v>
       </c>
-      <c r="C35" s="29">
-        <v>0</v>
-      </c>
-      <c r="D35" s="29">
+      <c r="C35" s="7">
+        <v>0</v>
+      </c>
+      <c r="D35" s="7">
         <v>0</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="29">
-        <v>0</v>
-      </c>
-      <c r="C36" s="29">
-        <v>0</v>
-      </c>
-      <c r="D36" s="29">
+      <c r="B36" s="7">
+        <v>0</v>
+      </c>
+      <c r="C36" s="7">
+        <v>0</v>
+      </c>
+      <c r="D36" s="7">
         <v>0</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="29">
-        <v>0</v>
-      </c>
-      <c r="C37" s="29">
-        <v>0</v>
-      </c>
-      <c r="D37" s="29">
+      <c r="B37" s="7">
+        <v>0</v>
+      </c>
+      <c r="C37" s="7">
+        <v>0</v>
+      </c>
+      <c r="D37" s="7">
         <v>0</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="29">
-        <v>0</v>
-      </c>
-      <c r="C38" s="29">
-        <v>0</v>
-      </c>
-      <c r="D38" s="29">
+      <c r="B38" s="7">
+        <v>0</v>
+      </c>
+      <c r="C38" s="7">
+        <v>0</v>
+      </c>
+      <c r="D38" s="7">
         <v>0</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B39" s="29">
-        <v>0</v>
-      </c>
-      <c r="C39" s="29">
-        <v>0</v>
-      </c>
-      <c r="D39" s="29">
+      <c r="B39" s="7">
+        <v>0</v>
+      </c>
+      <c r="C39" s="7">
+        <v>0</v>
+      </c>
+      <c r="D39" s="7">
         <v>0</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="29">
+      <c r="B40" s="7">
         <v>4</v>
       </c>
-      <c r="C40" s="29">
+      <c r="C40" s="7">
         <v>8</v>
       </c>
-      <c r="D40" s="29">
+      <c r="D40" s="7">
         <v>0</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="29">
+      <c r="B41" s="7">
         <v>2</v>
       </c>
-      <c r="C41" s="29">
-        <v>0</v>
-      </c>
-      <c r="D41" s="29">
+      <c r="C41" s="7">
+        <v>0</v>
+      </c>
+      <c r="D41" s="7">
         <v>0</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="29">
+      <c r="B42" s="7">
         <v>2</v>
       </c>
-      <c r="C42" s="29">
-        <v>0</v>
-      </c>
-      <c r="D42" s="29">
+      <c r="C42" s="7">
+        <v>0</v>
+      </c>
+      <c r="D42" s="7">
         <v>0</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="29">
-        <v>0</v>
-      </c>
-      <c r="C43" s="29">
+      <c r="B43" s="7">
+        <v>0</v>
+      </c>
+      <c r="C43" s="7">
         <v>8</v>
       </c>
-      <c r="D43" s="29">
+      <c r="D43" s="7">
         <v>0</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="30" t="s">
+      <c r="A44" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="B44" s="29">
-        <v>0</v>
-      </c>
-      <c r="C44" s="29">
+      <c r="B44" s="7">
+        <v>0</v>
+      </c>
+      <c r="C44" s="7">
         <v>8</v>
       </c>
-      <c r="D44" s="29">
+      <c r="D44" s="7">
         <v>0</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
     </row>
-    <row r="46" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="40" t="s">
+      <c r="C46" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D46" s="40" t="s">
+      <c r="D46" s="31" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="s">
+      <c r="A47" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B47" s="1">
@@ -3405,7 +3379,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B48" s="1">
@@ -3419,7 +3393,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B49" s="8">
@@ -3433,143 +3407,142 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="33"/>
-      <c r="B50" s="28"/>
-      <c r="C50" s="29"/>
+      <c r="A50" s="25"/>
+      <c r="C50" s="7"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="34"/>
-      <c r="D51" s="20"/>
+      <c r="B51" s="41"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="15"/>
     </row>
     <row r="52" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="B52" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C52" s="40" t="s">
+      <c r="C52" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D52" s="40" t="s">
+      <c r="D52" s="31" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="38" t="s">
+      <c r="A53" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="22">
+      <c r="B53" s="17">
         <v>1</v>
       </c>
       <c r="C53" s="8">
         <v>1</v>
       </c>
-      <c r="D53" s="22">
+      <c r="D53" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="37" t="s">
+      <c r="A54" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="19" t="s">
+      <c r="B54" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C54" s="40" t="s">
+      <c r="C54" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D54" s="40" t="s">
+      <c r="D54" s="31" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="35" t="s">
+      <c r="A55" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="35">
+      <c r="B55" s="26">
         <v>1</v>
       </c>
-      <c r="C55" s="35">
+      <c r="C55" s="26">
         <v>1</v>
       </c>
-      <c r="D55" s="21">
+      <c r="D55" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
+      <c r="A56" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B56" s="35">
+      <c r="B56" s="26">
         <v>2</v>
       </c>
-      <c r="C56" s="35">
+      <c r="C56" s="26">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D56" s="21">
+      <c r="D56" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B57" s="35">
+      <c r="B57" s="26">
         <v>1</v>
       </c>
-      <c r="C57" s="35">
+      <c r="C57" s="26">
         <v>1</v>
       </c>
-      <c r="D57" s="21">
+      <c r="D57" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="35" t="s">
+      <c r="A58" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B58" s="35">
+      <c r="B58" s="26">
         <v>1</v>
       </c>
-      <c r="C58" s="35">
-        <v>0</v>
-      </c>
-      <c r="D58" s="21">
+      <c r="C58" s="26">
+        <v>0</v>
+      </c>
+      <c r="D58" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="38" t="s">
+      <c r="A59" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B59" s="38">
-        <v>0</v>
-      </c>
-      <c r="C59" s="22">
-        <v>0</v>
-      </c>
-      <c r="D59" s="18">
+      <c r="B59" s="29">
+        <v>0</v>
+      </c>
+      <c r="C59" s="17">
+        <v>0</v>
+      </c>
+      <c r="D59" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="36"/>
+      <c r="A61" s="27"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
     </row>
     <row r="62" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B62" s="14"/>
-      <c r="C62" s="31"/>
-      <c r="D62" s="32"/>
+      <c r="B62" s="45"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="24"/>
     </row>
     <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
@@ -3579,7 +3552,7 @@
         <v>1</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="26"/>
+      <c r="D63" s="21"/>
     </row>
     <row r="64" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
@@ -3588,7 +3561,7 @@
       <c r="B64" s="1">
         <v>1</v>
       </c>
-      <c r="C64" s="16"/>
+      <c r="C64" s="11"/>
       <c r="D64" s="2"/>
     </row>
     <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3599,7 +3572,7 @@
         <v>1</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="26"/>
+      <c r="D65" s="21"/>
     </row>
     <row r="66" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
@@ -3608,43 +3581,42 @@
       <c r="B66" s="5">
         <v>1</v>
       </c>
-      <c r="C66" s="25"/>
+      <c r="C66" s="20"/>
       <c r="D66" s="6"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="30"/>
-      <c r="B67" s="28"/>
+      <c r="A67" s="23"/>
     </row>
     <row r="68" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="39" t="s">
+      <c r="A68" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="19" t="s">
+      <c r="B68" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C68" s="40" t="s">
+      <c r="C68" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D68" s="40" t="s">
+      <c r="D68" s="31" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="15" t="s">
+      <c r="A69" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B69" s="1">
         <v>2</v>
       </c>
-      <c r="C69" s="16">
+      <c r="C69" s="11">
         <v>3</v>
       </c>
-      <c r="D69" s="16">
+      <c r="D69" s="11">
         <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="15" t="s">
+      <c r="A70" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B70" s="1">
@@ -3653,26 +3625,26 @@
       <c r="C70" s="1">
         <v>1</v>
       </c>
-      <c r="D70" s="21">
+      <c r="D70" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
+      <c r="A71" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B71" s="1">
         <v>2</v>
       </c>
-      <c r="C71" s="16">
+      <c r="C71" s="11">
         <v>2</v>
       </c>
-      <c r="D71" s="16">
+      <c r="D71" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="15" t="s">
+      <c r="A72" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B72" s="1">
@@ -3681,35 +3653,35 @@
       <c r="C72" s="1">
         <v>1</v>
       </c>
-      <c r="D72" s="21">
+      <c r="D72" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
+      <c r="A73" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B73" s="8">
         <v>2</v>
       </c>
-      <c r="C73" s="18">
-        <v>0</v>
-      </c>
-      <c r="D73" s="18">
+      <c r="C73" s="13">
+        <v>0</v>
+      </c>
+      <c r="D73" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
+      <c r="A74" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B74" s="8">
         <v>0</v>
       </c>
-      <c r="C74" s="18">
-        <v>0</v>
-      </c>
-      <c r="D74" s="18">
+      <c r="C74" s="13">
+        <v>0</v>
+      </c>
+      <c r="D74" s="13">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add CBL17 (E1 loop) instead of RIC-E1
</commit_message>
<xml_diff>
--- a/Docs/BOM.ETX2i10G.xlsx
+++ b/Docs/BOM.ETX2i10G.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\ate\AutoTesters\TCL\ETX-2i-10G\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B443BF2-5D0D-4192-B961-BA1DE1E1F19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71802F20-888F-42AB-A2B3-B91B6C3AA89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38940" yWindow="1860" windowWidth="17025" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="345" windowWidth="20265" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="74">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -582,12 +582,18 @@
   <si>
     <t>order</t>
   </si>
+  <si>
+    <t>AT-ETX2i10G/CBL17</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -652,6 +658,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -991,7 +1004,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1098,6 +1111,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1125,6 +1139,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2365,8 +2380,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{29747EB6-9D7A-4AA7-AAD7-923DDA372A6C}" name="Table6" displayName="Table6" ref="A46:D49" totalsRowShown="0" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
-  <autoFilter ref="A46:D49" xr:uid="{29747EB6-9D7A-4AA7-AAD7-923DDA372A6C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{29747EB6-9D7A-4AA7-AAD7-923DDA372A6C}" name="Table6" displayName="Table6" ref="A47:D50" totalsRowShown="0" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+  <autoFilter ref="A47:D50" xr:uid="{29747EB6-9D7A-4AA7-AAD7-923DDA372A6C}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{479E1687-5AC7-4BA3-8758-214A4B6A5504}" name="4.       Mechanic parts:" dataDxfId="26"/>
     <tableColumn id="2" xr3:uid="{8252F755-5C3A-49F2-AB21-7657822BDCEE}" name=" 2 units" dataDxfId="25"/>
@@ -2378,8 +2393,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2940D1D2-1742-448B-BC6C-C654E9E16A3E}" name="Table7" displayName="Table7" ref="A54:D59" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
-  <autoFilter ref="A54:D59" xr:uid="{2940D1D2-1742-448B-BC6C-C654E9E16A3E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2940D1D2-1742-448B-BC6C-C654E9E16A3E}" name="Table7" displayName="Table7" ref="A55:D60" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+  <autoFilter ref="A55:D60" xr:uid="{2940D1D2-1742-448B-BC6C-C654E9E16A3E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{42289E71-A17F-4FD2-B9A7-AC6C60B88EC6}" name="5.2.    Movable equipment" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{E9E477FC-42DE-4DAD-A88A-A278C9AD03E0}" name=" 2 units" dataDxfId="16"/>
@@ -2391,8 +2406,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{308EC0D6-A130-4F10-9F7D-F559D1D64F90}" name="Table8" displayName="Table8" ref="A52:D53" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A52:D53" xr:uid="{308EC0D6-A130-4F10-9F7D-F559D1D64F90}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{308EC0D6-A130-4F10-9F7D-F559D1D64F90}" name="Table8" displayName="Table8" ref="A53:D54" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A53:D54" xr:uid="{308EC0D6-A130-4F10-9F7D-F559D1D64F90}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{83AF3E1C-0C53-4E3A-8FFB-089ED9175552}" name="5.1.    PC’s card" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{FA742A23-1518-4231-A7F2-20B45E8F818C}" name=" 2 units" dataDxfId="10"/>
@@ -2404,8 +2419,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{52632D65-FA75-4174-A90B-5C8B0A320A97}" name="Table9" displayName="Table9" ref="A68:D74" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="A68:D74" xr:uid="{52632D65-FA75-4174-A90B-5C8B0A320A97}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{52632D65-FA75-4174-A90B-5C8B0A320A97}" name="Table9" displayName="Table9" ref="A69:D75" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A69:D75" xr:uid="{52632D65-FA75-4174-A90B-5C8B0A320A97}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A60CF906-F771-47E1-92CE-46638A38F534}" name="7.       Miscellaneous:" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{5297B3B9-9B20-4BC3-9B9C-1B7F0C644436}" name=" 2 units" dataDxfId="2"/>
@@ -2679,10 +2694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2694,22 +2709,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="A2" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E3" s="37" t="s">
@@ -2719,7 +2734,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>62</v>
       </c>
@@ -2740,7 +2755,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="38" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="7">
@@ -2789,7 +2804,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="7">
-        <f t="shared" ref="C8:C56" si="0">B8*2</f>
+        <f t="shared" ref="C8:C57" si="0">B8*2</f>
         <v>4</v>
       </c>
       <c r="D8" s="7">
@@ -2838,7 +2853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>66</v>
       </c>
@@ -2913,14 +2928,14 @@
       <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="42"/>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="43"/>
+    </row>
+    <row r="18" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>61</v>
       </c>
@@ -2973,7 +2988,7 @@
       <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="48" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="7">
@@ -3069,7 +3084,7 @@
       <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="48" t="s">
         <v>37</v>
       </c>
       <c r="B27" s="7">
@@ -3090,7 +3105,7 @@
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
         <v>60</v>
       </c>
@@ -3350,338 +3365,362 @@
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
     </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
+    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="7">
+        <v>2</v>
+      </c>
+      <c r="C45" s="7">
+        <v>0</v>
+      </c>
+      <c r="D45" s="7">
+        <v>0</v>
+      </c>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="23"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B47" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="31" t="s">
+      <c r="C47" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D46" s="31" t="s">
+      <c r="D47" s="31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
+    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B48" s="1">
         <v>1</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C48" s="1">
         <v>1</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D48" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B49" s="1">
         <v>2</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C49" s="1">
         <v>2</v>
-      </c>
-      <c r="D48" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B49" s="8">
-        <v>2</v>
-      </c>
-      <c r="C49" s="1">
-        <v>0</v>
       </c>
       <c r="D49" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="25"/>
-      <c r="C50" s="7"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="40" t="s">
+    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="8">
+        <v>2</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="25"/>
+      <c r="C51" s="7"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B51" s="41"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="15"/>
-    </row>
-    <row r="52" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
+      <c r="B52" s="42"/>
+      <c r="C52" s="44"/>
+      <c r="D52" s="15"/>
+    </row>
+    <row r="53" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B53" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C52" s="31" t="s">
+      <c r="C53" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D52" s="31" t="s">
+      <c r="D53" s="31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="29" t="s">
+    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="17">
+      <c r="B54" s="17">
         <v>1</v>
       </c>
-      <c r="C53" s="8">
+      <c r="C54" s="8">
         <v>1</v>
       </c>
-      <c r="D53" s="17">
+      <c r="D54" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="s">
+    <row r="55" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B55" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C54" s="31" t="s">
+      <c r="C55" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D54" s="31" t="s">
+      <c r="D55" s="31" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B55" s="26">
-        <v>1</v>
-      </c>
-      <c r="C55" s="26">
-        <v>1</v>
-      </c>
-      <c r="D55" s="16">
-        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" s="26">
+        <v>1</v>
+      </c>
+      <c r="C56" s="26">
+        <v>1</v>
+      </c>
+      <c r="D56" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B56" s="26">
+      <c r="B57" s="26">
         <v>2</v>
       </c>
-      <c r="C56" s="26">
+      <c r="C57" s="26">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D56" s="16">
+      <c r="D57" s="16">
         <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="B57" s="26">
-        <v>1</v>
-      </c>
-      <c r="C57" s="26">
-        <v>1</v>
-      </c>
-      <c r="D57" s="16">
-        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="26" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="B58" s="26">
         <v>1</v>
       </c>
       <c r="C58" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="29" t="s">
+      <c r="A59" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B59" s="26">
+        <v>1</v>
+      </c>
+      <c r="C59" s="26">
+        <v>0</v>
+      </c>
+      <c r="D59" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B59" s="29">
-        <v>0</v>
-      </c>
-      <c r="C59" s="17">
-        <v>0</v>
-      </c>
-      <c r="D59" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="27"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-    </row>
-    <row r="62" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="44" t="s">
+      <c r="B60" s="29">
+        <v>0</v>
+      </c>
+      <c r="C60" s="17">
+        <v>0</v>
+      </c>
+      <c r="D60" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="27"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B62" s="45"/>
-      <c r="C62" s="46"/>
-      <c r="D62" s="24"/>
-    </row>
-    <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B63" s="1">
-        <v>1</v>
-      </c>
-      <c r="C63" s="1"/>
-      <c r="D63" s="21"/>
+      <c r="B63" s="46"/>
+      <c r="C63" s="47"/>
+      <c r="D63" s="24"/>
     </row>
     <row r="64" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="B64" s="1">
         <v>1</v>
       </c>
-      <c r="C64" s="11"/>
-      <c r="D64" s="2"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="21"/>
     </row>
     <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B65" s="1">
         <v>1</v>
       </c>
-      <c r="C65" s="1"/>
-      <c r="D65" s="21"/>
-    </row>
-    <row r="66" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
+      <c r="C65" s="11"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66" s="1">
+        <v>1</v>
+      </c>
+      <c r="C66" s="1"/>
+      <c r="D66" s="21"/>
+    </row>
+    <row r="67" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B66" s="5">
+      <c r="B67" s="5">
         <v>1</v>
       </c>
-      <c r="C66" s="20"/>
-      <c r="D66" s="6"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="23"/>
-    </row>
-    <row r="68" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="30" t="s">
+      <c r="C67" s="20"/>
+      <c r="D67" s="6"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="23"/>
+    </row>
+    <row r="69" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B69" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C68" s="31" t="s">
+      <c r="C69" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D68" s="31" t="s">
+      <c r="D69" s="31" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B69" s="1">
-        <v>2</v>
-      </c>
-      <c r="C69" s="11">
-        <v>3</v>
-      </c>
-      <c r="D69" s="11">
-        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B70" s="1">
-        <v>1</v>
-      </c>
-      <c r="C70" s="1">
-        <v>1</v>
-      </c>
-      <c r="D70" s="16">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C70" s="11">
+        <v>3</v>
+      </c>
+      <c r="D70" s="11">
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B71" s="1">
-        <v>2</v>
-      </c>
-      <c r="C71" s="11">
-        <v>2</v>
-      </c>
-      <c r="D71" s="11">
+        <v>1</v>
+      </c>
+      <c r="C71" s="1">
+        <v>1</v>
+      </c>
+      <c r="D71" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B72" s="1">
+        <v>2</v>
+      </c>
+      <c r="C72" s="11">
+        <v>2</v>
+      </c>
+      <c r="D72" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B73" s="1">
         <v>1</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C73" s="1">
         <v>1</v>
       </c>
-      <c r="D72" s="16">
+      <c r="D73" s="16">
         <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B73" s="8">
-        <v>2</v>
-      </c>
-      <c r="C73" s="13">
-        <v>0</v>
-      </c>
-      <c r="D73" s="13">
-        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B74" s="8">
+        <v>2</v>
+      </c>
+      <c r="C74" s="13">
+        <v>0</v>
+      </c>
+      <c r="D74" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B74" s="8">
-        <v>0</v>
-      </c>
-      <c r="C74" s="13">
-        <v>0</v>
-      </c>
-      <c r="D74" s="13">
+      <c r="B75" s="8">
+        <v>0</v>
+      </c>
+      <c r="C75" s="13">
+        <v>0</v>
+      </c>
+      <c r="D75" s="13">
         <v>2</v>
       </c>
     </row>
@@ -3690,15 +3729,15 @@
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="A63:C63"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="2" manualBreakCount="2">
     <brk id="27" max="16383" man="1"/>
-    <brk id="66" max="16383" man="1"/>
+    <brk id="67" max="16383" man="1"/>
   </rowBreaks>
   <tableParts count="8">
     <tablePart r:id="rId2"/>

</xml_diff>